<commit_message>
change name + logo + capture ecran
</commit_message>
<xml_diff>
--- a/public/samples/fichier_import_familles_et_membres.xlsx
+++ b/public/samples/fichier_import_familles_et_membres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\OneDrive\Bureau\Projets web\association\public\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287F99F0-02AE-4373-8866-291248774D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63336B02-A5E6-4F43-BE84-66A711669E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="468" windowWidth="21600" windowHeight="11292" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Familles" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
   <si>
     <t>typeFamille_nom</t>
   </si>
@@ -56,24 +56,6 @@
     <t>datePaiement</t>
   </si>
   <si>
-    <t>c7bf16e9-b340-4758-9a0b-da0b698d8101</t>
-  </si>
-  <si>
-    <t>699b889d-d281-45a1-acfd-d2f72d304f86</t>
-  </si>
-  <si>
-    <t>c71fad58-9fd1-4780-82c2-20add6705078</t>
-  </si>
-  <si>
-    <t>5d81ead1-aba1-4600-95e0-97f325c15aa0</t>
-  </si>
-  <si>
-    <t>493e87c1-704d-4031-9477-c95fad8b4844</t>
-  </si>
-  <si>
-    <t>2faf41b2-ff42-4a57-bb82-7290adb0f0f8</t>
-  </si>
-  <si>
     <t>Individuel</t>
   </si>
   <si>
@@ -288,9 +270,6 @@
   </si>
   <si>
     <t>familleChefPrenom</t>
-  </si>
-  <si>
-    <t>familleId</t>
   </si>
   <si>
     <t>nom</t>
@@ -783,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -826,334 +805,334 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <v>50</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H3">
         <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H4">
         <v>50</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H5">
         <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H6">
         <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H7">
         <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H8">
         <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H9">
         <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J9" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H11">
         <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="J11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="K11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1163,355 +1142,312 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>90</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D15" t="s">
         <v>97</v>
       </c>
-      <c r="F6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E15" t="s">
         <v>109</v>
       </c>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="F15" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" t="s">
-        <v>113</v>
-      </c>
-      <c r="G11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F14" t="s">
-        <v>115</v>
-      </c>
-      <c r="G14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" t="s">
-        <v>116</v>
-      </c>
-      <c r="G15" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>